<commit_message>
Fix bug of some stentence
</commit_message>
<xml_diff>
--- a/result/precision.xlsx
+++ b/result/precision.xlsx
@@ -3,13 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1225F648-F0E1-4F1C-AC15-CB127C097F0E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AFDA44-14F5-42AC-8128-A63E432F3934}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1:$A$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1:$B$4</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -126,16 +130,240 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0B2310E0-05AA-46A6-8B09-5C39C37E2319}" type="VALUE">
+                      <a:rPr lang="en-US" altLang="zh-CN">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr/>
+                      <a:t>[值]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-85B6-410C-A5D0-6677391EEC49}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2B0AFE6C-28BE-4535-8350-507F099B6565}" type="VALUE">
+                      <a:rPr lang="en-US" altLang="zh-CN">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr/>
+                      <a:t>[值]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-85B6-410C-A5D0-6677391EEC49}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FF0147FF-A520-4980-81B8-C173899CFDF3}" type="VALUE">
+                      <a:rPr lang="en-US" altLang="zh-CN">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr/>
+                      <a:t>[值]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-85B6-410C-A5D0-6677391EEC49}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="50000"/>
+                            <a:lumOff val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{A6A784D1-1870-4417-B1E6-D5AFA4AD2EA9}" type="VALUE">
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:schemeClr val="bg1"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[值]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:ln>
+                        <a:noFill/>
+                      </a:ln>
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-85B6-410C-A5D0-6677391EEC49}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -144,15 +372,19 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -175,14 +407,13 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                    <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -262,7 +493,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -272,6 +503,19 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -280,7 +524,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
+              <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -294,11 +538,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -327,7 +574,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="dk1">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -337,6 +584,19 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -344,11 +604,14 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -377,11 +640,14 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -399,14 +665,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -415,11 +675,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -435,17 +698,7 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:pattFill prst="ltDnDiag">
-          <a:fgClr>
-            <a:schemeClr val="dk1">
-              <a:lumMod val="15000"/>
-              <a:lumOff val="85000"/>
-            </a:schemeClr>
-          </a:fgClr>
-          <a:bgClr>
-            <a:schemeClr val="lt1"/>
-          </a:bgClr>
-        </a:pattFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -465,7 +718,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
@@ -478,7 +731,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="zh-CN"/>
     </a:p>
@@ -532,33 +789,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="303">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="301">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -566,9 +823,9 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -577,11 +834,11 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -596,9 +853,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -632,46 +889,62 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -683,31 +956,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="15875">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="2"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
@@ -726,23 +998,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="800" kern="1200"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -758,14 +1029,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -777,14 +1047,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -796,14 +1066,13 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -814,34 +1083,21 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -855,14 +1111,13 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -874,33 +1129,32 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -909,61 +1163,43 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -981,14 +1217,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -996,25 +1232,25 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="dk1">
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
         <a:lumMod val="50000"/>
         <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1026,9 +1262,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1044,14 +1280,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1060,22 +1295,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1085,19 +1309,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1106,16 +1317,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>331925</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>55079</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>103326</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>83654</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>629477</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>82825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1409,7 +1620,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>